<commit_message>
Second Year Grades updated
</commit_message>
<xml_diff>
--- a/DATA/Grades/Second Year/1st Year/1st Sem/BSIT 1C_IT 103 .xlsx
+++ b/DATA/Grades/Second Year/1st Year/1st Sem/BSIT 1C_IT 103 .xlsx
@@ -74,7 +74,7 @@
   </commentList>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mjhyOlFAmbICuljQ4SQKSe2vj8zOQ=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mhUgg9flzW5sc1Ul5PMf1Mx09V4Sw=="/>
     </ext>
   </extLst>
 </comments>
@@ -1249,6 +1249,9 @@
     <xf borderId="22" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
+    <xf borderId="22" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="23" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="23" fillId="0" fontId="9" numFmtId="1" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -1284,9 +1287,6 @@
     </xf>
     <xf borderId="23" fillId="0" fontId="9" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="22" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -1560,7 +1560,7 @@
     <xdr:ext cx="914400" cy="914400"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png"/>
+        <xdr:cNvPr id="0" name="image2.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1588,7 +1588,7 @@
     <xdr:ext cx="914400" cy="914400"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png"/>
+        <xdr:cNvPr id="0" name="image1.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1621,7 +1621,7 @@
     <xdr:ext cx="914400" cy="914400"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png"/>
+        <xdr:cNvPr id="0" name="image2.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1649,7 +1649,7 @@
     <xdr:ext cx="914400" cy="914400"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png"/>
+        <xdr:cNvPr id="0" name="image1.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2680,30 +2680,30 @@
       <c r="E17" s="54"/>
       <c r="F17" s="55">
         <f t="shared" si="1"/>
-        <v>2.25</v>
-      </c>
-      <c r="G17" s="56">
-        <v>78.0</v>
+        <v>2.5</v>
+      </c>
+      <c r="G17" s="68">
+        <v>50.0</v>
       </c>
       <c r="H17" s="56">
         <v>60.0</v>
       </c>
-      <c r="I17" s="56">
-        <v>120.0</v>
+      <c r="I17" s="68">
+        <v>90.0</v>
       </c>
       <c r="J17" s="57">
         <f t="shared" si="2"/>
-        <v>79.31818182</v>
-      </c>
-      <c r="K17" s="56">
-        <v>41.0</v>
+        <v>72.72727273</v>
+      </c>
+      <c r="K17" s="68">
+        <v>36.0</v>
       </c>
       <c r="L17" s="56">
         <v>30.0</v>
       </c>
       <c r="M17" s="58">
         <f t="shared" si="3"/>
-        <v>79.58333333</v>
+        <v>77.5</v>
       </c>
       <c r="N17" s="59">
         <v>2.0</v>
@@ -2728,20 +2728,20 @@
       <c r="T17" s="67">
         <v>63.0</v>
       </c>
-      <c r="U17" s="67">
-        <v>88.0</v>
+      <c r="U17" s="64">
+        <v>66.0</v>
       </c>
       <c r="V17" s="65">
         <f t="shared" si="6"/>
-        <v>87.75</v>
+        <v>82.25</v>
       </c>
       <c r="W17" s="66">
         <f t="shared" si="7"/>
-        <v>84.46831387</v>
+        <v>80.42437448</v>
       </c>
       <c r="X17" s="66">
         <f>VLOOKUP(W17,'Grade Range'!$A$2:$B$11,2)</f>
-        <v>2.25</v>
+        <v>2.5</v>
       </c>
       <c r="Y17" s="66" t="str">
         <f t="shared" si="8"/>
@@ -3868,7 +3868,7 @@
       <c r="E31" s="54"/>
       <c r="F31" s="55">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>2.25</v>
       </c>
       <c r="G31" s="56">
         <v>70.0</v>
@@ -3876,12 +3876,12 @@
       <c r="H31" s="56">
         <v>70.0</v>
       </c>
-      <c r="I31" s="56">
-        <v>199.0</v>
+      <c r="I31" s="68">
+        <v>150.0</v>
       </c>
       <c r="J31" s="57">
         <f t="shared" si="2"/>
-        <v>88.52272727</v>
+        <v>82.95454545</v>
       </c>
       <c r="K31" s="56">
         <v>32.0</v>
@@ -3916,20 +3916,20 @@
       <c r="T31" s="67">
         <v>66.0</v>
       </c>
-      <c r="U31" s="67">
-        <v>86.0</v>
+      <c r="U31" s="64">
+        <v>69.0</v>
       </c>
       <c r="V31" s="65">
         <f t="shared" si="6"/>
-        <v>88</v>
+        <v>83.75</v>
       </c>
       <c r="W31" s="66">
         <f t="shared" si="7"/>
-        <v>87.45376008</v>
+        <v>84.50830553</v>
       </c>
       <c r="X31" s="66">
         <f>VLOOKUP(W31,'Grade Range'!$A$2:$B$11,2)</f>
-        <v>2</v>
+        <v>2.25</v>
       </c>
       <c r="Y31" s="66" t="str">
         <f t="shared" si="8"/>
@@ -5043,89 +5043,89 @@
       <c r="Z44" s="66"/>
     </row>
     <row r="45" ht="12.0" customHeight="1">
-      <c r="A45" s="68">
+      <c r="A45" s="69">
         <v>33.0</v>
       </c>
-      <c r="B45" s="68" t="s">
+      <c r="B45" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="C45" s="69">
+      <c r="C45" s="70">
         <v>2.021114942E9</v>
       </c>
-      <c r="D45" s="70" t="s">
+      <c r="D45" s="71" t="s">
         <v>58</v>
       </c>
-      <c r="E45" s="70"/>
-      <c r="F45" s="71">
+      <c r="E45" s="71"/>
+      <c r="F45" s="72">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="G45" s="72">
+      <c r="G45" s="73">
         <v>63.0</v>
       </c>
-      <c r="H45" s="72">
+      <c r="H45" s="73">
         <v>100.0</v>
       </c>
-      <c r="I45" s="72">
+      <c r="I45" s="73">
         <v>177.0</v>
       </c>
-      <c r="J45" s="73">
+      <c r="J45" s="74">
         <f t="shared" si="2"/>
         <v>88.63636364</v>
       </c>
-      <c r="K45" s="72">
+      <c r="K45" s="73">
         <v>39.0</v>
       </c>
-      <c r="L45" s="72">
+      <c r="L45" s="73">
         <v>31.0</v>
       </c>
-      <c r="M45" s="74">
+      <c r="M45" s="75">
         <f t="shared" si="3"/>
         <v>79.16666667</v>
       </c>
-      <c r="N45" s="75">
+      <c r="N45" s="76">
         <v>2.0</v>
       </c>
-      <c r="O45" s="75">
+      <c r="O45" s="76">
         <v>7.0</v>
       </c>
-      <c r="P45" s="75">
+      <c r="P45" s="76">
         <v>85.0</v>
       </c>
-      <c r="Q45" s="76">
+      <c r="Q45" s="77">
         <f t="shared" si="4"/>
         <v>93.11926606</v>
       </c>
-      <c r="R45" s="77">
+      <c r="R45" s="78">
         <v>5.0</v>
       </c>
-      <c r="S45" s="78">
+      <c r="S45" s="79">
         <f t="shared" si="5"/>
         <v>75</v>
       </c>
-      <c r="T45" s="79">
+      <c r="T45" s="80">
         <v>86.0</v>
       </c>
-      <c r="U45" s="79">
+      <c r="U45" s="80">
         <v>74.0</v>
       </c>
-      <c r="V45" s="80">
+      <c r="V45" s="81">
         <f t="shared" si="6"/>
         <v>90</v>
       </c>
-      <c r="W45" s="81">
+      <c r="W45" s="82">
         <f t="shared" si="7"/>
         <v>87.14213233</v>
       </c>
-      <c r="X45" s="81">
+      <c r="X45" s="82">
         <f>VLOOKUP(W45,'Grade Range'!$A$2:$B$11,2)</f>
         <v>2</v>
       </c>
-      <c r="Y45" s="81" t="str">
+      <c r="Y45" s="82" t="str">
         <f t="shared" si="8"/>
         <v>Passed</v>
       </c>
-      <c r="Z45" s="81"/>
+      <c r="Z45" s="82"/>
     </row>
     <row r="46" ht="12.0" customHeight="1">
       <c r="A46" s="52">
@@ -5246,7 +5246,7 @@
       <c r="K47" s="56">
         <v>30.0</v>
       </c>
-      <c r="L47" s="82">
+      <c r="L47" s="68">
         <v>33.0</v>
       </c>
       <c r="M47" s="58">
@@ -5993,7 +5993,7 @@
       <c r="E56" s="54"/>
       <c r="F56" s="55">
         <f t="shared" si="1"/>
-        <v>2.25</v>
+        <v>2.5</v>
       </c>
       <c r="G56" s="56">
         <v>91.0</v>
@@ -6001,12 +6001,12 @@
       <c r="H56" s="56">
         <v>112.0</v>
       </c>
-      <c r="I56" s="56">
-        <v>173.0</v>
+      <c r="I56" s="68">
+        <v>100.0</v>
       </c>
       <c r="J56" s="57">
         <f t="shared" si="2"/>
-        <v>92.72727273</v>
+        <v>84.43181818</v>
       </c>
       <c r="K56" s="56">
         <v>42.0</v>
@@ -6050,11 +6050,11 @@
       </c>
       <c r="W56" s="66">
         <f t="shared" si="7"/>
-        <v>83.54088824</v>
+        <v>81.05225188</v>
       </c>
       <c r="X56" s="66">
         <f>VLOOKUP(W56,'Grade Range'!$A$2:$B$11,2)</f>
-        <v>2.25</v>
+        <v>2.5</v>
       </c>
       <c r="Y56" s="66" t="str">
         <f t="shared" si="8"/>
@@ -6333,30 +6333,30 @@
       <c r="E60" s="54"/>
       <c r="F60" s="55">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="G60" s="56">
-        <v>104.0</v>
+        <v>2.25</v>
+      </c>
+      <c r="G60" s="68">
+        <v>85.0</v>
       </c>
       <c r="H60" s="56">
         <v>72.0</v>
       </c>
-      <c r="I60" s="56">
-        <v>150.0</v>
+      <c r="I60" s="68">
+        <v>90.0</v>
       </c>
       <c r="J60" s="57">
         <f t="shared" si="2"/>
-        <v>87.04545455</v>
-      </c>
-      <c r="K60" s="56">
-        <v>52.0</v>
+        <v>78.06818182</v>
+      </c>
+      <c r="K60" s="68">
+        <v>45.0</v>
       </c>
       <c r="L60" s="56">
         <v>42.0</v>
       </c>
       <c r="M60" s="58">
         <f t="shared" si="3"/>
-        <v>89.16666667</v>
+        <v>86.25</v>
       </c>
       <c r="N60" s="59">
         <v>2.0</v>
@@ -6381,20 +6381,20 @@
       <c r="T60" s="67">
         <v>52.0</v>
       </c>
-      <c r="U60" s="67">
-        <v>91.0</v>
+      <c r="U60" s="64">
+        <v>65.0</v>
       </c>
       <c r="V60" s="65">
         <f t="shared" si="6"/>
-        <v>85.75</v>
+        <v>79.25</v>
       </c>
       <c r="W60" s="66">
         <f t="shared" si="7"/>
-        <v>87.95866694</v>
+        <v>82.73215179</v>
       </c>
       <c r="X60" s="66">
         <f>VLOOKUP(W60,'Grade Range'!$A$2:$B$11,2)</f>
-        <v>2</v>
+        <v>2.25</v>
       </c>
       <c r="Y60" s="66" t="str">
         <f t="shared" si="8"/>

</xml_diff>